<commit_message>
Fixed setting end dates for viranomaispaatos and kompostori
- Fixed setting end dates for viranomaispaatos and kompostori if alkupvm <= expiring kohde loppupvm.
- Adjusted tests.
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/ilmoitukset.xlsx
+++ b/tests/data/test_data_import/ilmoitukset.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="113">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -332,6 +332,33 @@
   </si>
   <si>
     <t xml:space="preserve">Yksittäinen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.6.2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uusi ilmoitus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karita</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyykoski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0400123645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">karita@pyykoski.fi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karita Pyykoski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kyykoski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iivari</t>
   </si>
 </sst>
 </file>
@@ -343,7 +370,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -385,11 +412,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -445,7 +467,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -486,10 +508,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -507,15 +525,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT2"/>
+  <dimension ref="A1:BT3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -803,16 +927,16 @@
       <c r="R2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="V2" s="10" t="s">
+      <c r="S2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="9" t="s">
         <v>83</v>
       </c>
       <c r="W2" s="1" t="s">
@@ -896,13 +1020,13 @@
       <c r="BA2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BB2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC2" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD2" s="10" t="s">
+      <c r="BB2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD2" s="9" t="s">
         <v>83</v>
       </c>
       <c r="BE2" s="1" t="s">
@@ -914,16 +1038,184 @@
       <c r="BQ2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BR2" s="11" t="n">
+      <c r="BR2" s="10" t="n">
         <v>46398.0000011574</v>
       </c>
       <c r="BT2" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AW3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AX3" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="AY3" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR3" s="10" t="n">
+        <v>46398.0000011574</v>
+      </c>
+      <c r="BT3" s="1" t="s">
         <v>103</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="johan@kemp.fi"/>
+    <hyperlink ref="G3" r:id="rId2" display="karita@pyykoski.fi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Add updating kohde in KompostorinKohteet
- Update KompostorinKohteet when Ilmoitus affects new kohde.
- Update KohteenOsapuoli when Ilmoitus affects new kohde.
- Adjusted tests.
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/ilmoitukset.xlsx
+++ b/tests/data/test_data_import/ilmoitukset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -353,12 +353,6 @@
   </si>
   <si>
     <t xml:space="preserve">Karita Pyykoski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyykoski</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iivari</t>
   </si>
 </sst>
 </file>
@@ -638,7 +632,7 @@
   </sheetPr>
   <dimension ref="A1:BT3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
     </sheetView>
   </sheetViews>
@@ -1083,7 +1077,7 @@
         <v>81</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="P3" s="9" t="s">
         <v>79</v>
@@ -1173,10 +1167,10 @@
         <v>100</v>
       </c>
       <c r="AW3" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="AX3" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="AY3" s="9" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Fix the bug when updating kohteet and kompostori has multiple kohde
</commit_message>
<xml_diff>
--- a/tests/data/test_data_import/ilmoitukset.xlsx
+++ b/tests/data/test_data_import/ilmoitukset.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="116">
   <si>
     <t xml:space="preserve">Vastausaika</t>
   </si>
@@ -346,13 +346,28 @@
     <t xml:space="preserve">Pyykoski</t>
   </si>
   <si>
+    <t xml:space="preserve">Karita Pyykoski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forsström</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kuvakalliontie 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100456789B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kimppa</t>
+  </si>
+  <si>
     <t xml:space="preserve">0400123645</t>
   </si>
   <si>
     <t xml:space="preserve">karita@pyykoski.fi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Karita Pyykoski</t>
   </si>
 </sst>
 </file>
@@ -364,7 +379,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -406,6 +421,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -461,7 +481,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -506,6 +526,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,121 +543,15 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="LibreOffice">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="000000"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="ffffff"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="18a303"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="0369a3"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a33e03"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8e03a3"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="c99c00"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="c9211e"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000ee"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="551a8b"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BT3"/>
+  <dimension ref="A1:BT4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1056,10 +974,10 @@
         <v>107</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>79</v>
@@ -1071,7 +989,7 @@
         <v>81</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>81</v>
@@ -1163,17 +1081,17 @@
       <c r="AU3" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AV3" s="1" t="s">
-        <v>100</v>
+      <c r="AV3" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="AW3" s="9" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AX3" s="9" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="AY3" s="9" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="AZ3" s="2" t="s">
         <v>80</v>
@@ -1181,14 +1099,14 @@
       <c r="BA3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BB3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="BD3" s="9" t="s">
-        <v>83</v>
+      <c r="BB3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="BD3" s="11" t="s">
+        <v>112</v>
       </c>
       <c r="BE3" s="1" t="s">
         <v>101</v>
@@ -1203,13 +1121,181 @@
         <v>46398.0000011574</v>
       </c>
       <c r="BT3" s="1" t="s">
-        <v>103</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="P4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="1" t="n">
+        <v>160</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AP4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AV4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW4" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AX4" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AY4" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="BA4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BB4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BC4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BD4" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="BF4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ4" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="BR4" s="10" t="n">
+        <v>46398.0000011574</v>
+      </c>
+      <c r="BT4" s="1" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" display="johan@kemp.fi"/>
-    <hyperlink ref="G3" r:id="rId2" display="karita@pyykoski.fi"/>
+    <hyperlink ref="G3" r:id="rId2" display="johan@kemp.fi"/>
+    <hyperlink ref="G4" r:id="rId3" display="karita@pyykoski.fi"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>